<commit_message>
caracteristicas switches y tipos de comunicacion
</commit_message>
<xml_diff>
--- a/docs/ccna2.xlsx
+++ b/docs/ccna2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-v19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23877170-C15D-4CCB-8006-9311A39832F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C90619-110B-4D21-9E60-0038A7E1FDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>TIA-568A</t>
   </si>
@@ -149,6 +149,111 @@
   </si>
   <si>
     <t>&lt;= 2km</t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>Simplex</t>
+  </si>
+  <si>
+    <t>Half Duplex</t>
+  </si>
+  <si>
+    <t>Full Duplex</t>
+  </si>
+  <si>
+    <t>Full Full Duplex</t>
+  </si>
+  <si>
+    <t>un host envia o recibe datos</t>
+  </si>
+  <si>
+    <t>un host envia y el resto recibe</t>
+  </si>
+  <si>
+    <t>un host envia y recibe datos</t>
+  </si>
+  <si>
+    <t>varios hosts envian y reciben</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Metodo</t>
+  </si>
+  <si>
+    <t>Config. Fija</t>
+  </si>
+  <si>
+    <t>Modular</t>
+  </si>
+  <si>
+    <t>Apilable</t>
+  </si>
+  <si>
+    <t>Pueden aumentar su capacidad, con modulos de expansion que soportan distintas interfaces.</t>
+  </si>
+  <si>
+    <t>Permite utilizar dos o mas dispositivos como si uno de mayor capacidad.</t>
+  </si>
+  <si>
+    <t>Cantidad de puertos limitada, son accesibles y se recomiendan para la capa de acceso.</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Cut-through</t>
+  </si>
+  <si>
+    <t>Store-N-Forward</t>
+  </si>
+  <si>
+    <t>Fragment-Free</t>
+  </si>
+  <si>
+    <t>runt</t>
+  </si>
+  <si>
+    <t>giant</t>
+  </si>
+  <si>
+    <t>throttle</t>
+  </si>
+  <si>
+    <t>crc</t>
+  </si>
+  <si>
+    <t>Trama</t>
+  </si>
+  <si>
+    <t>miden menos de 64 Bytes</t>
+  </si>
+  <si>
+    <t>miden mas de 1500 Bytes</t>
+  </si>
+  <si>
+    <t>descartada por desbordamiento</t>
+  </si>
+  <si>
+    <t>errores de verificacion de trama</t>
+  </si>
+  <si>
+    <t>El dispositivo reenvia la trama apenas identifica la direccion MAC de Destino.</t>
+  </si>
+  <si>
+    <t>Almacenan la trama en un buffer de memoria y una vez controlada, realizan el reenvio.</t>
+  </si>
+  <si>
+    <t>Verifican los primeros 64Bytes de la trama, antes de realizar el reenvio de la misma.</t>
+  </si>
+  <si>
+    <t>Colision</t>
   </si>
 </sst>
 </file>
@@ -232,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,11 +366,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -507,6 +625,50 @@
     <tableColumn id="1" xr3:uid="{811CF7CB-AF7A-49A4-B931-B5A5776276B0}" name="Fibra"/>
     <tableColumn id="2" xr3:uid="{6E816054-8584-42F4-B34C-FA4E92F9FBBF}" name="SMF"/>
     <tableColumn id="3" xr3:uid="{40EEA95C-A97B-408A-8B89-C69D1DB8C03A}" name="MMF"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{430A0DF1-18CE-419E-88FE-CBF9967144E3}" name="Tabla2" displayName="Tabla2" ref="A7:B10" totalsRowShown="0">
+  <autoFilter ref="A7:B10" xr:uid="{430A0DF1-18CE-419E-88FE-CBF9967144E3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{63601882-E000-48DA-A02A-BAA511CE762A}" name="Switch"/>
+    <tableColumn id="2" xr3:uid="{21909B7A-D274-431D-8476-10BFBC128559}" name="Caracteristica" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AF04FD3A-FB8D-49DE-846A-33E9CBC792AE}" name="Tabla4" displayName="Tabla4" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{AF04FD3A-FB8D-49DE-846A-33E9CBC792AE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{74736B2F-755A-4B48-AB7B-0B239F5F6E2F}" name="Comunicación"/>
+    <tableColumn id="2" xr3:uid="{C076C465-1236-427F-B4F9-4DA4036C02B6}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EE48087A-B43E-41F8-B1FE-3435FAA78917}" name="Tabla5" displayName="Tabla5" ref="D1:E5" totalsRowShown="0">
+  <autoFilter ref="D1:E5" xr:uid="{EE48087A-B43E-41F8-B1FE-3435FAA78917}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{20451D20-3FCE-4274-856A-6DA3991626A4}" name="Colision"/>
+    <tableColumn id="2" xr3:uid="{8723FB01-AD60-443F-96DF-A5E4611B3AB5}" name="Trama"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CCC662FD-AF2B-4AB9-9E2C-C8FB9D1EFD8A}" name="Tabla6" displayName="Tabla6" ref="D7:E10" totalsRowShown="0">
+  <autoFilter ref="D7:E10" xr:uid="{CCC662FD-AF2B-4AB9-9E2C-C8FB9D1EFD8A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{75AAB5BC-0DF3-4049-B52F-41349869B4AC}" name="Metodo" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{813739C1-473B-4058-BC52-F59C259A5CDA}" name="Descripcion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -811,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735A3117-379D-4818-B537-9985464A7E52}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,12 +1176,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825BE79D-83FE-4953-B272-787464DD8696}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
señalizacion y problemas capa fisica
</commit_message>
<xml_diff>
--- a/docs/ccna2.xlsx
+++ b/docs/ccna2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-v19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C90619-110B-4D21-9E60-0038A7E1FDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB1A95B-5CAF-413C-8B9B-1DADC828D678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
   </bookViews>
   <sheets>
     <sheet name="Fisica" sheetId="1" r:id="rId1"/>
     <sheet name="Enlace" sheetId="2" r:id="rId2"/>
+    <sheet name="Red" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>TIA-568A</t>
   </si>
@@ -254,13 +255,55 @@
   </si>
   <si>
     <t>Colision</t>
+  </si>
+  <si>
+    <t>Problemas</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>CrossTalk</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Señal</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada (Rango)</t>
+  </si>
+  <si>
+    <t>Frecuencia Modulada (Ciclos)</t>
+  </si>
+  <si>
+    <t>Fase Modulada (2 Señales)</t>
+  </si>
+  <si>
+    <t>Interferencia Electromagnetica</t>
+  </si>
+  <si>
+    <t>Diafonia (cruce de señales)</t>
+  </si>
+  <si>
+    <t>Interferencia Radiofrecuencial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +311,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +375,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -333,11 +396,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,24 +447,59 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -401,15 +517,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>544286</xdr:colOff>
+      <xdr:colOff>551793</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>59872</xdr:colOff>
+      <xdr:colOff>52552</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>125186</xdr:rowOff>
+      <xdr:rowOff>59121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -424,13 +540,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="544286" y="272143"/>
-          <a:ext cx="870857" cy="424543"/>
+          <a:off x="551793" y="216776"/>
+          <a:ext cx="853966" cy="413845"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="38100">
           <a:solidFill>
             <a:schemeClr val="accent6">
               <a:lumMod val="40000"/>
@@ -459,15 +575,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>522515</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:rowOff>39414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>32658</xdr:colOff>
+      <xdr:colOff>52552</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:rowOff>91966</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -482,12 +598,19 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="522515" y="451757"/>
-          <a:ext cx="865414" cy="756557"/>
+          <a:off x="571500" y="420414"/>
+          <a:ext cx="834259" cy="814552"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="3">
@@ -509,15 +632,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>582386</xdr:colOff>
+      <xdr:colOff>551793</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:rowOff>78828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>59872</xdr:colOff>
+      <xdr:colOff>78827</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
+      <xdr:rowOff>157655</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -532,17 +655,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="582386" y="288471"/>
-          <a:ext cx="832757" cy="375558"/>
+          <a:off x="551793" y="269328"/>
+          <a:ext cx="880241" cy="459827"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="38100">
           <a:solidFill>
             <a:schemeClr val="accent2">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
@@ -567,15 +690,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>544286</xdr:colOff>
+      <xdr:colOff>532086</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:rowOff>144518</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>32658</xdr:colOff>
+      <xdr:colOff>13138</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>125187</xdr:rowOff>
+      <xdr:rowOff>85397</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -590,13 +713,19 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="544286" y="468086"/>
-          <a:ext cx="843643" cy="800101"/>
+          <a:off x="532086" y="525518"/>
+          <a:ext cx="834259" cy="702879"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="3">
@@ -616,62 +745,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{51767F72-1A39-4BF8-A55E-7F61A81F087E}" name="Tabla1" displayName="Tabla1" ref="E1:G9" totalsRowShown="0">
-  <autoFilter ref="E1:G9" xr:uid="{51767F72-1A39-4BF8-A55E-7F61A81F087E}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{811CF7CB-AF7A-49A4-B931-B5A5776276B0}" name="Fibra"/>
-    <tableColumn id="2" xr3:uid="{6E816054-8584-42F4-B34C-FA4E92F9FBBF}" name="SMF"/>
-    <tableColumn id="3" xr3:uid="{40EEA95C-A97B-408A-8B89-C69D1DB8C03A}" name="MMF"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{430A0DF1-18CE-419E-88FE-CBF9967144E3}" name="Tabla2" displayName="Tabla2" ref="A7:B10" totalsRowShown="0">
-  <autoFilter ref="A7:B10" xr:uid="{430A0DF1-18CE-419E-88FE-CBF9967144E3}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63601882-E000-48DA-A02A-BAA511CE762A}" name="Switch"/>
-    <tableColumn id="2" xr3:uid="{21909B7A-D274-431D-8476-10BFBC128559}" name="Caracteristica" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AF04FD3A-FB8D-49DE-846A-33E9CBC792AE}" name="Tabla4" displayName="Tabla4" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{AF04FD3A-FB8D-49DE-846A-33E9CBC792AE}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{74736B2F-755A-4B48-AB7B-0B239F5F6E2F}" name="Comunicación"/>
-    <tableColumn id="2" xr3:uid="{C076C465-1236-427F-B4F9-4DA4036C02B6}" name="Descripcion"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EE48087A-B43E-41F8-B1FE-3435FAA78917}" name="Tabla5" displayName="Tabla5" ref="D1:E5" totalsRowShown="0">
-  <autoFilter ref="D1:E5" xr:uid="{EE48087A-B43E-41F8-B1FE-3435FAA78917}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{20451D20-3FCE-4274-856A-6DA3991626A4}" name="Colision"/>
-    <tableColumn id="2" xr3:uid="{8723FB01-AD60-443F-96DF-A5E4611B3AB5}" name="Trama"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CCC662FD-AF2B-4AB9-9E2C-C8FB9D1EFD8A}" name="Tabla6" displayName="Tabla6" ref="D7:E10" totalsRowShown="0">
-  <autoFilter ref="D7:E10" xr:uid="{CCC662FD-AF2B-4AB9-9E2C-C8FB9D1EFD8A}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{75AAB5BC-0DF3-4049-B52F-41349869B4AC}" name="Metodo" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{813739C1-473B-4058-BC52-F59C259A5CDA}" name="Descripcion"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -971,11 +1044,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735A3117-379D-4818-B537-9985464A7E52}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -985,9 +1056,12 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -995,17 +1069,23 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1015,17 +1095,23 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1035,17 +1121,23 @@
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1055,17 +1147,23 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1075,17 +1173,17 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -1095,17 +1193,23 @@
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1115,17 +1219,23 @@
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1135,17 +1245,23 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1155,22 +1271,25 @@
       <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="12" t="s">
         <v>34</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -1178,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825BE79D-83FE-4953-B272-787464DD8696}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,139 +1310,148 @@
     <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="25" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="29" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD1F744-D77F-4CBB-8295-477903A7A8B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dominios de difusion y colision
</commit_message>
<xml_diff>
--- a/docs/ccna2.xlsx
+++ b/docs/ccna2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-v19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB1A95B-5CAF-413C-8B9B-1DADC828D678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5150C7A8-A867-47F7-BB71-1FE897D60640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
   </bookViews>
@@ -1046,7 +1046,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735A3117-379D-4818-B537-9985464A7E52}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1298,7 +1300,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
enrutamiento estatico y configuracion hsrp
</commit_message>
<xml_diff>
--- a/docs/ccna2.xlsx
+++ b/docs/ccna2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-v19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D3970A-835D-4DC0-819C-1A929DA45F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC376C36-A09C-475B-BF03-FF83D816C4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="6" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{97D4C5BA-1F41-4457-9F13-C02AA4365D66}"/>
   </bookViews>
   <sheets>
     <sheet name="Fisica" sheetId="1" r:id="rId1"/>
@@ -1404,13 +1404,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1450,6 +1444,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2710,7 +2710,10 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
-          <a:endParaRPr lang="es-AR"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>115</a:t>
+          </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2827,6 +2830,45 @@
           <a:r>
             <a:rPr lang="es-AR"/>
             <a:t>110</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>Desconocida</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DD6EE715-96D1-423A-8625-623AFF7FAA9B}" type="parTrans" cxnId="{DA70A1AA-7E63-4541-B81E-302C783961DE}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FB5E9BAF-C5EC-4F08-9C5B-D4BFF951308C}" type="sibTrans" cxnId="{DA70A1AA-7E63-4541-B81E-302C783961DE}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>255</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2875,7 +2917,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AB60E39D-4D9D-42A3-8B1D-410FB9A75302}" type="pres">
-      <dgm:prSet presAssocID="{0F17D45C-7A25-4F18-8D1A-6D35E0E22B7D}" presName="rootConnector1" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="15"/>
+      <dgm:prSet presAssocID="{0F17D45C-7A25-4F18-8D1A-6D35E0E22B7D}" presName="rootConnector1" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="16"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{85895A5F-4636-4B35-B0ED-D14BFED6A8E5}" type="pres">
@@ -2883,7 +2925,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{182BF4BA-552D-4299-A17F-3EA29EB65A12}" type="pres">
-      <dgm:prSet presAssocID="{5484BCC3-0749-4041-96BA-412A07C81BFB}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:prSet presAssocID="{5484BCC3-0749-4041-96BA-412A07C81BFB}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="3"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8B6928AB-C246-43E0-A2CF-55FF8571A458}" type="pres">
@@ -2899,7 +2941,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8BB2ECB5-8860-4FF5-BD2E-BA2B6AB7761F}" type="pres">
-      <dgm:prSet presAssocID="{22E82712-0C2F-4F1A-A0A5-CA396ED69428}" presName="rootText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="15">
+      <dgm:prSet presAssocID="{22E82712-0C2F-4F1A-A0A5-CA396ED69428}" presName="rootText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -2908,7 +2950,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{2A52CE97-DB2A-42C7-9BA3-F3E78ED94EE7}" type="pres">
-      <dgm:prSet presAssocID="{22E82712-0C2F-4F1A-A0A5-CA396ED69428}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="0" presStyleCnt="15">
+      <dgm:prSet presAssocID="{22E82712-0C2F-4F1A-A0A5-CA396ED69428}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="0" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2941,7 +2983,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{4FF18F15-D939-4B2B-84BC-6CA83CE8B574}" type="pres">
-      <dgm:prSet presAssocID="{1FBFD739-E8E6-4692-8EE7-CC824EF5F064}" presName="rootText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="15">
+      <dgm:prSet presAssocID="{1FBFD739-E8E6-4692-8EE7-CC824EF5F064}" presName="rootText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -2950,7 +2992,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F6C42163-BA6F-4B07-BC1F-8D682BFF80FC}" type="pres">
-      <dgm:prSet presAssocID="{1FBFD739-E8E6-4692-8EE7-CC824EF5F064}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="1" presStyleCnt="15">
+      <dgm:prSet presAssocID="{1FBFD739-E8E6-4692-8EE7-CC824EF5F064}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="1" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2987,7 +3029,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{2A88E684-6F3F-49FE-A756-CCD64EF04752}" type="pres">
-      <dgm:prSet presAssocID="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" presName="rootText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="15">
+      <dgm:prSet presAssocID="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" presName="rootText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -2996,7 +3038,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{04F63F44-ACB3-4DDB-965B-CE33A8B944CE}" type="pres">
-      <dgm:prSet presAssocID="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="2" presStyleCnt="15">
+      <dgm:prSet presAssocID="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="2" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3021,7 +3063,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F5A5C269-41AA-45A1-92FC-C0539B927B51}" type="pres">
-      <dgm:prSet presAssocID="{7C509599-E8CD-4F74-9BFE-9460D76D2216}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:prSet presAssocID="{7C509599-E8CD-4F74-9BFE-9460D76D2216}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="3"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7D508C1A-A9D5-4DA4-B1CB-0CC9ADCF41D4}" type="pres">
@@ -3037,7 +3079,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{0E02854D-3334-4D61-B237-C3E8F474D727}" type="pres">
-      <dgm:prSet presAssocID="{11D54C12-4976-4DE1-AA97-025725F50CC1}" presName="rootText" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="15">
+      <dgm:prSet presAssocID="{11D54C12-4976-4DE1-AA97-025725F50CC1}" presName="rootText" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3046,7 +3088,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{B3EBC84C-4A53-473F-B54E-95230E39FB12}" type="pres">
-      <dgm:prSet presAssocID="{11D54C12-4976-4DE1-AA97-025725F50CC1}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="3" presStyleCnt="15">
+      <dgm:prSet presAssocID="{11D54C12-4976-4DE1-AA97-025725F50CC1}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="3" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3079,7 +3121,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{59208A25-FF93-43CA-8D1C-2E75A4D45C45}" type="pres">
-      <dgm:prSet presAssocID="{DA6AC9ED-7878-4ECE-B323-31E7461BD817}" presName="rootText" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="15">
+      <dgm:prSet presAssocID="{DA6AC9ED-7878-4ECE-B323-31E7461BD817}" presName="rootText" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3088,7 +3130,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{84D89B8F-8A10-4ADF-9BF6-50A074007891}" type="pres">
-      <dgm:prSet presAssocID="{DA6AC9ED-7878-4ECE-B323-31E7461BD817}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="4" presStyleCnt="15">
+      <dgm:prSet presAssocID="{DA6AC9ED-7878-4ECE-B323-31E7461BD817}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="4" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3125,7 +3167,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{47971EDD-A107-4ADF-8DED-721559CD573D}" type="pres">
-      <dgm:prSet presAssocID="{10303D85-4DF8-46FB-ABB2-376F62A93969}" presName="rootText" presStyleLbl="node1" presStyleIdx="5" presStyleCnt="15">
+      <dgm:prSet presAssocID="{10303D85-4DF8-46FB-ABB2-376F62A93969}" presName="rootText" presStyleLbl="node1" presStyleIdx="5" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3134,7 +3176,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{0E427561-B050-464B-A7FC-E055024E44F1}" type="pres">
-      <dgm:prSet presAssocID="{10303D85-4DF8-46FB-ABB2-376F62A93969}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="5" presStyleCnt="15">
+      <dgm:prSet presAssocID="{10303D85-4DF8-46FB-ABB2-376F62A93969}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="5" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3167,7 +3209,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7C623FA2-0882-4901-9D44-C5856BB410E5}" type="pres">
-      <dgm:prSet presAssocID="{9F25A638-EDF9-4598-B5E4-8BB9F262F2E4}" presName="rootText" presStyleLbl="node1" presStyleIdx="6" presStyleCnt="15">
+      <dgm:prSet presAssocID="{9F25A638-EDF9-4598-B5E4-8BB9F262F2E4}" presName="rootText" presStyleLbl="node1" presStyleIdx="6" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3176,7 +3218,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{24AD543A-B2CE-469D-80C8-05DA0BB408A3}" type="pres">
-      <dgm:prSet presAssocID="{9F25A638-EDF9-4598-B5E4-8BB9F262F2E4}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="6" presStyleCnt="15">
+      <dgm:prSet presAssocID="{9F25A638-EDF9-4598-B5E4-8BB9F262F2E4}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="6" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3209,7 +3251,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{599A8A27-5248-41C6-9560-830BC57005F0}" type="pres">
-      <dgm:prSet presAssocID="{EADB60BD-279C-438B-8CE7-7376DC6243BD}" presName="rootText" presStyleLbl="node1" presStyleIdx="7" presStyleCnt="15">
+      <dgm:prSet presAssocID="{EADB60BD-279C-438B-8CE7-7376DC6243BD}" presName="rootText" presStyleLbl="node1" presStyleIdx="7" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3218,7 +3260,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AB37844F-1263-465B-ACB8-BFBEA32E7D43}" type="pres">
-      <dgm:prSet presAssocID="{EADB60BD-279C-438B-8CE7-7376DC6243BD}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="7" presStyleCnt="15">
+      <dgm:prSet presAssocID="{EADB60BD-279C-438B-8CE7-7376DC6243BD}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="7" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3251,7 +3293,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{39D46A10-2F82-40F9-948F-F526A6771473}" type="pres">
-      <dgm:prSet presAssocID="{59BFC301-431D-497D-8ACF-661789085CB4}" presName="rootText" presStyleLbl="node1" presStyleIdx="8" presStyleCnt="15">
+      <dgm:prSet presAssocID="{59BFC301-431D-497D-8ACF-661789085CB4}" presName="rootText" presStyleLbl="node1" presStyleIdx="8" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3260,7 +3302,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{E660B803-2EA0-4B8A-8935-FF821193CA08}" type="pres">
-      <dgm:prSet presAssocID="{59BFC301-431D-497D-8ACF-661789085CB4}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="8" presStyleCnt="15">
+      <dgm:prSet presAssocID="{59BFC301-431D-497D-8ACF-661789085CB4}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="8" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3297,7 +3339,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{A4085EEF-D86A-479B-B346-B23DCDFBF324}" type="pres">
-      <dgm:prSet presAssocID="{B64305BA-3AE0-4050-AEF2-B66B14A69660}" presName="rootText" presStyleLbl="node1" presStyleIdx="9" presStyleCnt="15">
+      <dgm:prSet presAssocID="{B64305BA-3AE0-4050-AEF2-B66B14A69660}" presName="rootText" presStyleLbl="node1" presStyleIdx="9" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3306,7 +3348,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{280B24DE-6CF3-42BE-A670-3B09647C024A}" type="pres">
-      <dgm:prSet presAssocID="{B64305BA-3AE0-4050-AEF2-B66B14A69660}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="9" presStyleCnt="15">
+      <dgm:prSet presAssocID="{B64305BA-3AE0-4050-AEF2-B66B14A69660}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="9" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3347,7 +3389,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F8CFD625-6FD6-4A73-A6BC-3E50C03CC3F1}" type="pres">
-      <dgm:prSet presAssocID="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" presName="rootText" presStyleLbl="node1" presStyleIdx="10" presStyleCnt="15">
+      <dgm:prSet presAssocID="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" presName="rootText" presStyleLbl="node1" presStyleIdx="10" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3356,7 +3398,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{503C61C0-1370-4FCD-85BE-070AAC8875D6}" type="pres">
-      <dgm:prSet presAssocID="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="10" presStyleCnt="15">
+      <dgm:prSet presAssocID="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="10" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3389,7 +3431,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AA7C5249-4279-4AFD-9A53-13E2E9516AF2}" type="pres">
-      <dgm:prSet presAssocID="{B93C0E95-0FAF-4E29-8468-9CDDEE2C56C3}" presName="rootText" presStyleLbl="node1" presStyleIdx="11" presStyleCnt="15">
+      <dgm:prSet presAssocID="{B93C0E95-0FAF-4E29-8468-9CDDEE2C56C3}" presName="rootText" presStyleLbl="node1" presStyleIdx="11" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3398,7 +3440,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{34DB4A73-9398-4C69-9D05-6FDE9791D972}" type="pres">
-      <dgm:prSet presAssocID="{B93C0E95-0FAF-4E29-8468-9CDDEE2C56C3}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="11" presStyleCnt="15">
+      <dgm:prSet presAssocID="{B93C0E95-0FAF-4E29-8468-9CDDEE2C56C3}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="11" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3435,7 +3477,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{C567307D-799E-4200-AFF2-1F0C0E0D8DC3}" type="pres">
-      <dgm:prSet presAssocID="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" presName="rootText" presStyleLbl="node1" presStyleIdx="12" presStyleCnt="15">
+      <dgm:prSet presAssocID="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" presName="rootText" presStyleLbl="node1" presStyleIdx="12" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3444,7 +3486,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{212441E6-928E-4A2B-A6FE-15AFD7A5E823}" type="pres">
-      <dgm:prSet presAssocID="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="12" presStyleCnt="15">
+      <dgm:prSet presAssocID="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="12" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3489,7 +3531,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{6CD73B39-3008-456C-BF5C-0094245A608C}" type="pres">
-      <dgm:prSet presAssocID="{1C7B4D81-8299-4C93-82CE-52B2F8BB388F}" presName="rootText" presStyleLbl="node1" presStyleIdx="13" presStyleCnt="15">
+      <dgm:prSet presAssocID="{1C7B4D81-8299-4C93-82CE-52B2F8BB388F}" presName="rootText" presStyleLbl="node1" presStyleIdx="13" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3498,7 +3540,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{E55C164A-D158-44C3-992D-9E05203EC78A}" type="pres">
-      <dgm:prSet presAssocID="{1C7B4D81-8299-4C93-82CE-52B2F8BB388F}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="13" presStyleCnt="15">
+      <dgm:prSet presAssocID="{1C7B4D81-8299-4C93-82CE-52B2F8BB388F}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="13" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3531,7 +3573,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F53E32E6-1B95-4DC0-8746-5EC314B7E0ED}" type="pres">
-      <dgm:prSet presAssocID="{A1D8CE79-365D-4ED1-A882-444B0674D685}" presName="rootText" presStyleLbl="node1" presStyleIdx="14" presStyleCnt="15">
+      <dgm:prSet presAssocID="{A1D8CE79-365D-4ED1-A882-444B0674D685}" presName="rootText" presStyleLbl="node1" presStyleIdx="14" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax/>
           <dgm:chPref val="3"/>
@@ -3540,7 +3582,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{71CEC9A2-8043-42B2-8F31-BF0E6BE9F92A}" type="pres">
-      <dgm:prSet presAssocID="{A1D8CE79-365D-4ED1-A882-444B0674D685}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="14" presStyleCnt="15">
+      <dgm:prSet presAssocID="{A1D8CE79-365D-4ED1-A882-444B0674D685}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="14" presStyleCnt="16">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3572,6 +3614,52 @@
       <dgm:prSet presAssocID="{11D54C12-4976-4DE1-AA97-025725F50CC1}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{04CBAFCF-382E-4D8F-A667-F070920A71BB}" type="pres">
+      <dgm:prSet presAssocID="{DD6EE715-96D1-423A-8625-623AFF7FAA9B}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="3"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DAC6FEC0-1915-409C-9C78-92CEAC95AD59}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E75C26DB-7B8F-4F10-8A9E-BCEB7F16F730}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9B6B8576-2E1F-4286-BDE0-9C8BAC7DBD7E}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="rootText" presStyleLbl="node1" presStyleIdx="15" presStyleCnt="16">
+        <dgm:presLayoutVars>
+          <dgm:chMax/>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{18CBFCD1-65B0-495C-8F36-17F65655C045}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="titleText2" presStyleLbl="fgAcc1" presStyleIdx="15" presStyleCnt="16">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:chPref val="0"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{76516A00-6D79-4145-9D8C-F1C82CC23E87}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2BFC6478-4CF8-428B-A618-AC34446FB0D5}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{760B8948-5A79-46B2-9F1C-DCE464D9A72D}" type="pres">
+      <dgm:prSet presAssocID="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{94D2B33B-2975-4035-B9CD-421D9ACFAD2D}" type="pres">
       <dgm:prSet presAssocID="{0F17D45C-7A25-4F18-8D1A-6D35E0E22B7D}" presName="hierChild3" presStyleCnt="0"/>
       <dgm:spPr/>
@@ -3580,12 +3668,14 @@
   <dgm:cxnLst>
     <dgm:cxn modelId="{67666904-ECE2-4525-A343-4C73585CFB6B}" type="presOf" srcId="{59BFC301-431D-497D-8ACF-661789085CB4}" destId="{1C7DBA5D-F539-4037-BD20-A04FFFDE70BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{E1382D05-5F93-4ECA-89FF-57560872CDF5}" type="presOf" srcId="{1C7B4D81-8299-4C93-82CE-52B2F8BB388F}" destId="{6CD73B39-3008-456C-BF5C-0094245A608C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{0765EA05-7119-4C74-B92C-C38D0861C69A}" type="presOf" srcId="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" destId="{9B6B8576-2E1F-4286-BDE0-9C8BAC7DBD7E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{D4063106-7A6E-4977-9BAD-FEAF5082A80F}" type="presOf" srcId="{B64305BA-3AE0-4050-AEF2-B66B14A69660}" destId="{E3C1CAA6-CEA2-49FF-A601-A0213252A39A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{01583906-742C-45C2-A17A-42A44AAB0771}" type="presOf" srcId="{B680C1F1-D06C-4ED1-976F-FA2BE9714D89}" destId="{B3EBC84C-4A53-473F-B54E-95230E39FB12}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{CC56EA0D-B118-4210-90FE-07F89DE6C37D}" type="presOf" srcId="{DA6AC9ED-7878-4ECE-B323-31E7461BD817}" destId="{1DF1F81C-8976-44F8-A227-D95D2F8B14B4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{16EA2110-BC1A-43EC-AC36-DB93A8CF39CD}" type="presOf" srcId="{7FFA0F2C-E1C4-4B01-B7D8-A7DEC6061A55}" destId="{0EAD125B-9D67-487F-88F4-6249CAA88FD3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{C4A63610-4A6E-4614-BB26-3244F16C3CD8}" type="presOf" srcId="{84E86F0E-1405-4075-AB3C-F363865DDBFD}" destId="{71CEC9A2-8043-42B2-8F31-BF0E6BE9F92A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{A6FC7012-06E3-4CC1-9D59-A81EE3984B4E}" srcId="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" destId="{B93C0E95-0FAF-4E29-8468-9CDDEE2C56C3}" srcOrd="0" destOrd="0" parTransId="{97E19506-BBB1-4A1A-9B70-E7F881BB7329}" sibTransId="{8537B541-5D6B-4069-84E0-083D9F8B1B9E}"/>
+    <dgm:cxn modelId="{D1B49613-011E-43ED-9B5C-5C7EB7E4D433}" type="presOf" srcId="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" destId="{76516A00-6D79-4145-9D8C-F1C82CC23E87}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{910E3714-EF01-43A3-BFEE-F5019AD9E354}" type="presOf" srcId="{2B27202D-9D7C-4D81-90F6-8CCB4C9547EE}" destId="{212441E6-928E-4A2B-A6FE-15AFD7A5E823}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{87E9C916-CF9B-45D2-8D27-099B0AA34071}" type="presOf" srcId="{7120203A-0EE5-44B1-985A-63B8DFF414F8}" destId="{334374A4-66AF-48AD-B280-A3C0F52D1EB4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{14C2891C-3D5B-4E9F-8EFE-F8217F5264CE}" type="presOf" srcId="{F33C11F5-F428-4865-88A6-030B28779F1B}" destId="{8AA02455-D6DD-4A52-8DE6-4A4F1493B03F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
@@ -3625,6 +3715,8 @@
     <dgm:cxn modelId="{4E209BA0-9420-4F6F-8D98-86E32440A76D}" type="presOf" srcId="{9F25A638-EDF9-4598-B5E4-8BB9F262F2E4}" destId="{D0DED5E0-2708-44C2-A6F1-7F441A69F5B0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{DEE938A8-FD49-4792-AE83-1DC8BB8EB808}" srcId="{9DD1B3CD-980F-4657-A6A7-6B516FDAD8B2}" destId="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" srcOrd="1" destOrd="0" parTransId="{3C3436D8-6857-4A95-BB2E-980283C3FB7F}" sibTransId="{2B27202D-9D7C-4D81-90F6-8CCB4C9547EE}"/>
     <dgm:cxn modelId="{BD5B7EA9-ECFA-48E1-9FF5-116D21791EF3}" type="presOf" srcId="{0B04A615-B070-4E57-824F-005869DFF1BE}" destId="{12007E61-601B-42F2-9E81-4421C9B0BA5E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{DA70A1AA-7E63-4541-B81E-302C783961DE}" srcId="{0F17D45C-7A25-4F18-8D1A-6D35E0E22B7D}" destId="{7849090C-94CD-49FF-BDF8-0348E9EC76FB}" srcOrd="2" destOrd="0" parTransId="{DD6EE715-96D1-423A-8625-623AFF7FAA9B}" sibTransId="{FB5E9BAF-C5EC-4F08-9C5B-D4BFF951308C}"/>
+    <dgm:cxn modelId="{146C13AF-FB99-45C8-AB2A-603216D01EDE}" type="presOf" srcId="{DD6EE715-96D1-423A-8625-623AFF7FAA9B}" destId="{04CBAFCF-382E-4D8F-A667-F070920A71BB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{2FCCB1AF-FEA0-42C6-ADEF-8940FADD8508}" type="presOf" srcId="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" destId="{CF513147-89FB-4A12-9FBC-DD5ABBFAF254}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{02D72DB1-AA08-40B1-B67C-EB480D0BC51D}" type="presOf" srcId="{C00EA9CB-824A-45E1-B2C5-B09098C02A2C}" destId="{2A88E684-6F3F-49FE-A756-CCD64EF04752}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{FA7172B1-629A-4CCD-8DF3-F3C77117BF21}" type="presOf" srcId="{3C3436D8-6857-4A95-BB2E-980283C3FB7F}" destId="{404AD5B3-CE8D-4D2C-8E7A-AE901B111CC5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
@@ -3654,6 +3746,7 @@
     <dgm:cxn modelId="{360DFEEA-7CD7-450E-99ED-40FF041A9974}" type="presOf" srcId="{5484BCC3-0749-4041-96BA-412A07C81BFB}" destId="{182BF4BA-552D-4299-A17F-3EA29EB65A12}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{F8C905ED-652F-44AD-B97C-C293858FE8AC}" srcId="{EADB60BD-279C-438B-8CE7-7376DC6243BD}" destId="{59BFC301-431D-497D-8ACF-661789085CB4}" srcOrd="0" destOrd="0" parTransId="{0B04A615-B070-4E57-824F-005869DFF1BE}" sibTransId="{FB00BFE8-51F7-445F-97C9-15C72E72C9CD}"/>
     <dgm:cxn modelId="{80B2F6F0-4A3A-4F39-BDE4-7E129D78EAA6}" type="presOf" srcId="{0AB7532C-2D98-4A56-8E5B-AF3AD1D58652}" destId="{617D29DC-C6F8-4D7B-84DF-2DEE75D122F0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{09492EF2-F965-45D7-8627-319524A04BF4}" type="presOf" srcId="{FB5E9BAF-C5EC-4F08-9C5B-D4BFF951308C}" destId="{18CBFCD1-65B0-495C-8F36-17F65655C045}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{46176BF2-D723-44BF-9B05-8A31F51C0667}" type="presOf" srcId="{7E0A99B1-017F-4E50-B5B5-A3F6EF990FFC}" destId="{C567307D-799E-4200-AFF2-1F0C0E0D8DC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{E4BBAFF5-BBC2-4786-ACE9-00D7847AC1C2}" type="presOf" srcId="{0EEC3464-F0E1-49B7-A74C-CFBD2D77D8B8}" destId="{B9DC69DE-CB9F-4941-9B7B-7B092BB5076F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{CFE113F6-3AF1-4893-A3B7-26B9934AA6D1}" type="presOf" srcId="{22E82712-0C2F-4F1A-A0A5-CA396ED69428}" destId="{0E640679-51A8-400A-BE52-378E63EA2B94}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
@@ -3784,6 +3877,14 @@
     <dgm:cxn modelId="{C45F67C1-BBC2-44A8-A6AE-45B1EB6CAB9F}" type="presParOf" srcId="{79BE4581-9295-4BD3-82D8-6DD432E195FA}" destId="{42160415-F873-4A52-8E77-756E87264EA3}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{F3DE44D3-7853-4E2A-BA57-82BCA7D7290E}" type="presParOf" srcId="{5C730B16-769A-44B0-8383-2BBBD8FAD543}" destId="{B5477C54-C626-4060-817E-09FDD06C3CA3}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{5406D936-1680-4F55-AA87-7C67CAA0BC47}" type="presParOf" srcId="{7D508C1A-A9D5-4DA4-B1CB-0CC9ADCF41D4}" destId="{2000ECD1-761A-4B93-A671-88E31A610987}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{8D45C627-ADD6-4DE4-9DDC-0F6BA284C4C8}" type="presParOf" srcId="{85895A5F-4636-4B35-B0ED-D14BFED6A8E5}" destId="{04CBAFCF-382E-4D8F-A667-F070920A71BB}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{7AEB40EB-F59F-44B3-800C-0DA717EF81B8}" type="presParOf" srcId="{85895A5F-4636-4B35-B0ED-D14BFED6A8E5}" destId="{DAC6FEC0-1915-409C-9C78-92CEAC95AD59}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{9A0707F9-4437-4703-9224-9DA996E10DB6}" type="presParOf" srcId="{DAC6FEC0-1915-409C-9C78-92CEAC95AD59}" destId="{E75C26DB-7B8F-4F10-8A9E-BCEB7F16F730}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{849C85D7-ABB7-4AF4-B812-59F0E4BB5F2F}" type="presParOf" srcId="{E75C26DB-7B8F-4F10-8A9E-BCEB7F16F730}" destId="{9B6B8576-2E1F-4286-BDE0-9C8BAC7DBD7E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{D32DAF7C-587B-49C1-A121-44BE7D75B2A6}" type="presParOf" srcId="{E75C26DB-7B8F-4F10-8A9E-BCEB7F16F730}" destId="{18CBFCD1-65B0-495C-8F36-17F65655C045}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{546AEDF2-932C-467A-8863-A617895B3BB0}" type="presParOf" srcId="{E75C26DB-7B8F-4F10-8A9E-BCEB7F16F730}" destId="{76516A00-6D79-4145-9D8C-F1C82CC23E87}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{C1B0292F-1FEF-44D4-80C4-7081E5FD4EAB}" type="presParOf" srcId="{DAC6FEC0-1915-409C-9C78-92CEAC95AD59}" destId="{2BFC6478-4CF8-428B-A618-AC34446FB0D5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
+    <dgm:cxn modelId="{56D3F2EA-C602-4411-92C6-67505E0E7089}" type="presParOf" srcId="{DAC6FEC0-1915-409C-9C78-92CEAC95AD59}" destId="{760B8948-5A79-46B2-9F1C-DCE464D9A72D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
     <dgm:cxn modelId="{DF5E7079-E195-417F-8350-623B7E06C2D5}" type="presParOf" srcId="{0559FC95-7605-451F-8EDF-2AEAC7EC9A5D}" destId="{94D2B33B-2975-4035-B9CD-421D9ACFAD2D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/NameandTitleOrganizationalChart"/>
   </dgm:cxnLst>
   <dgm:bg/>
@@ -3804,6 +3905,68 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
+    <dsp:sp modelId="{04CBAFCF-382E-4D8F-A667-F070920A71BB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2257520" y="305354"/>
+          <a:ext cx="1184090" cy="176015"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="104932"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1184090" y="104932"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1184090" y="176015"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
     <dsp:sp modelId="{0EAD125B-9D67-487F-88F4-6249CAA88FD3}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
@@ -3811,8 +3974,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3789010" y="1747170"/>
-          <a:ext cx="91440" cy="175942"/>
+          <a:off x="3790587" y="1747324"/>
+          <a:ext cx="91440" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3826,7 +3989,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="175942"/>
+                <a:pt x="45720" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3867,8 +4030,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3045661" y="1266711"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="3046914" y="1266667"/>
+          <a:ext cx="789393" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3882,13 +4045,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="789393" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="175942"/>
+                <a:pt x="789393" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3929,8 +4092,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3045661" y="2227629"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="3046914" y="2227981"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3944,13 +4107,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="175942"/>
+                <a:pt x="394696" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3991,8 +4154,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2651127" y="2227629"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="2652217" y="2227981"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4003,16 +4166,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="394534" y="0"/>
+                <a:pt x="394696" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4053,8 +4216,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2256592" y="1747170"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="2257520" y="1747324"/>
+          <a:ext cx="789393" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4068,13 +4231,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="789393" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="175942"/>
+                <a:pt x="789393" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4115,8 +4278,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1467523" y="2227629"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="1468127" y="2227981"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4130,13 +4293,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="175942"/>
+                <a:pt x="394696" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4177,8 +4340,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1072989" y="2227629"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="1073430" y="2227981"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4189,16 +4352,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="394534" y="0"/>
+                <a:pt x="394696" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4239,8 +4402,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1467523" y="1747170"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="1468127" y="1747324"/>
+          <a:ext cx="789393" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4251,16 +4414,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="789068" y="0"/>
+                <a:pt x="789393" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="789393" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4301,8 +4464,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2256592" y="1266711"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="2257520" y="1266667"/>
+          <a:ext cx="789393" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4313,16 +4476,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="789068" y="0"/>
+                <a:pt x="789393" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="789393" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4363,8 +4526,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2651127" y="786252"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="2652217" y="786011"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4378,13 +4541,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="175942"/>
+                <a:pt x="394696" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4425,8 +4588,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2256592" y="786252"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="2257520" y="786011"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4437,16 +4600,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="394534" y="0"/>
+                <a:pt x="394696" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4487,8 +4650,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1862058" y="305792"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="2257520" y="305354"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4502,13 +4665,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="789068" y="175942"/>
+                <a:pt x="394696" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4549,8 +4712,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1072989" y="786252"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="1073430" y="786011"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4564,13 +4727,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="394534" y="175942"/>
+                <a:pt x="394696" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4611,8 +4774,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="678454" y="786252"/>
-          <a:ext cx="394534" cy="175942"/>
+          <a:off x="678733" y="786011"/>
+          <a:ext cx="394696" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4623,16 +4786,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="394534" y="0"/>
+                <a:pt x="394696" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="394534" y="104888"/>
+                <a:pt x="394696" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4673,8 +4836,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1072989" y="305792"/>
-          <a:ext cx="789068" cy="175942"/>
+          <a:off x="1073430" y="305354"/>
+          <a:ext cx="1184090" cy="176015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4685,16 +4848,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="789068" y="0"/>
+                <a:pt x="1184090" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="789068" y="104888"/>
+                <a:pt x="1184090" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="104888"/>
+                <a:pt x="0" y="104932"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="175942"/>
+                <a:pt x="0" y="176015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4735,8 +4898,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1567984" y="1276"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1963326" y="713"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4778,12 +4941,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4796,14 +4959,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>IP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1567984" y="1276"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1963326" y="713"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8AA02455-D6DD-4A52-8DE6-4A4F1493B03F}">
@@ -4813,8 +4976,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1685614" y="238122"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2081004" y="237656"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4876,8 +5039,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1685614" y="238122"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2081004" y="237656"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8BB2ECB5-8860-4FF5-BD2E-BA2B6AB7761F}">
@@ -4887,8 +5050,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="778915" y="481735"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="779236" y="481369"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4930,12 +5093,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4948,14 +5111,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Local</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="778915" y="481735"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="779236" y="481369"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2A52CE97-DB2A-42C7-9BA3-F3E78ED94EE7}">
@@ -4965,8 +5128,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="896545" y="718581"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="896913" y="718313"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5031,8 +5194,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="896545" y="718581"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="896913" y="718313"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4FF18F15-D939-4B2B-84BC-6CA83CE8B574}">
@@ -5042,8 +5205,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="384381" y="962194"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="384539" y="962026"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5085,12 +5248,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5103,14 +5266,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Interfaz</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="384381" y="962194"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="384539" y="962026"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F6C42163-BA6F-4B07-BC1F-8D682BFF80FC}">
@@ -5120,8 +5283,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="502010" y="1199040"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="502217" y="1198969"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5186,8 +5349,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="502010" y="1199040"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="502217" y="1198969"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2A88E684-6F3F-49FE-A756-CCD64EF04752}">
@@ -5197,8 +5360,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1173450" y="962194"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1173932" y="962026"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5240,12 +5403,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5258,14 +5421,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Red Conectada</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1173450" y="962194"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1173932" y="962026"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{04F63F44-ACB3-4DDB-965B-CE33A8B944CE}">
@@ -5275,8 +5438,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1291079" y="1199040"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="1291610" y="1198969"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5341,8 +5504,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1291079" y="1199040"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="1291610" y="1198969"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0E02854D-3334-4D61-B237-C3E8F474D727}">
@@ -5352,8 +5515,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2357053" y="481735"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="2358023" y="481369"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5395,12 +5558,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5413,14 +5576,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Remoto</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2357053" y="481735"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="2358023" y="481369"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B3EBC84C-4A53-473F-B54E-95230E39FB12}">
@@ -5430,8 +5593,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2474683" y="718581"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2475700" y="718313"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5496,8 +5659,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2474683" y="718581"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2475700" y="718313"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{59208A25-FF93-43CA-8D1C-2E75A4D45C45}">
@@ -5507,8 +5670,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1962519" y="962194"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1963326" y="962026"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5550,12 +5713,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5568,14 +5731,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Estatica</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1962519" y="962194"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1963326" y="962026"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{84D89B8F-8A10-4ADF-9BF6-50A074007891}">
@@ -5585,8 +5748,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2080148" y="1199040"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2081004" y="1198969"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5651,8 +5814,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2080148" y="1199040"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2081004" y="1198969"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{47971EDD-A107-4ADF-8DED-721559CD573D}">
@@ -5662,8 +5825,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2751588" y="962194"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="2752719" y="962026"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5705,12 +5868,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5723,14 +5886,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Dinamica</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2751588" y="962194"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="2752719" y="962026"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0E427561-B050-464B-A7FC-E055024E44F1}">
@@ -5740,8 +5903,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2869217" y="1199040"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2870397" y="1198969"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5803,8 +5966,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2869217" y="1199040"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2870397" y="1198969"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7C623FA2-0882-4901-9D44-C5856BB410E5}">
@@ -5814,8 +5977,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1962519" y="1442653"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1963326" y="1442683"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5857,12 +6020,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5875,14 +6038,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>IGP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1962519" y="1442653"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1963326" y="1442683"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{24AD543A-B2CE-469D-80C8-05DA0BB408A3}">
@@ -5892,8 +6055,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2080148" y="1679499"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2081004" y="1679626"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5955,8 +6118,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2080148" y="1679499"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2081004" y="1679626"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{599A8A27-5248-41C6-9560-830BC57005F0}">
@@ -5966,8 +6129,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1173450" y="1923112"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1173932" y="1923339"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6009,12 +6172,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6027,14 +6190,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>Link-state</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1173450" y="1923112"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1173932" y="1923339"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AB37844F-1263-465B-ACB8-BFBEA32E7D43}">
@@ -6044,8 +6207,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1291079" y="2159958"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="1291610" y="2160283"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6107,8 +6270,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1291079" y="2159958"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="1291610" y="2160283"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{39D46A10-2F82-40F9-948F-F526A6771473}">
@@ -6118,8 +6281,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="778915" y="2403571"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="779236" y="2403996"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6161,12 +6324,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6179,14 +6342,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>IS-IS</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="778915" y="2403571"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="779236" y="2403996"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E660B803-2EA0-4B8A-8935-FF821193CA08}">
@@ -6196,8 +6359,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="896545" y="2640417"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="896913" y="2640939"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6255,12 +6418,15 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="es-AR" sz="600" kern="1200"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="600" kern="1200"/>
+            <a:t>115</a:t>
+          </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="896545" y="2640417"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="896913" y="2640939"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A4085EEF-D86A-479B-B346-B23DCDFBF324}">
@@ -6270,8 +6436,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1567984" y="2403571"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="1568629" y="2403996"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6313,12 +6479,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6331,14 +6497,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>OSPF</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1567984" y="2403571"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="1568629" y="2403996"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{280B24DE-6CF3-42BE-A670-3B09647C024A}">
@@ -6348,8 +6514,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1685614" y="2640417"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="1686307" y="2640939"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6414,8 +6580,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1685614" y="2640417"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="1686307" y="2640939"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F8CFD625-6FD6-4A73-A6BC-3E50C03CC3F1}">
@@ -6425,8 +6591,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2751588" y="1923112"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="2752719" y="1923339"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6468,12 +6634,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6486,14 +6652,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>vector-distance</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2751588" y="1923112"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="2752719" y="1923339"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{503C61C0-1370-4FCD-85BE-070AAC8875D6}">
@@ -6503,8 +6669,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2869217" y="2159958"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2870397" y="2160283"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6566,8 +6732,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2869217" y="2159958"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2870397" y="2160283"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AA7C5249-4279-4AFD-9A53-13E2E9516AF2}">
@@ -6577,8 +6743,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2357053" y="2403571"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="2358023" y="2403996"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6620,12 +6786,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6638,14 +6804,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>RIP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2357053" y="2403571"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="2358023" y="2403996"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{34DB4A73-9398-4C69-9D05-6FDE9791D972}">
@@ -6655,8 +6821,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2474683" y="2640417"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="2475700" y="2640939"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6721,8 +6887,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2474683" y="2640417"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="2475700" y="2640939"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C567307D-799E-4200-AFF2-1F0C0E0D8DC3}">
@@ -6732,8 +6898,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3146122" y="2403571"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="3147416" y="2403996"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6775,12 +6941,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6793,14 +6959,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>EIGRP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3146122" y="2403571"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="3147416" y="2403996"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{212441E6-928E-4A2B-A6FE-15AFD7A5E823}">
@@ -6810,8 +6976,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3263752" y="2640417"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="3265094" y="2640939"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6876,8 +7042,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3263752" y="2640417"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="3265094" y="2640939"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6CD73B39-3008-456C-BF5C-0094245A608C}">
@@ -6887,8 +7053,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3540657" y="1442653"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="3542113" y="1442683"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6930,12 +7096,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6948,14 +7114,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>EGP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3540657" y="1442653"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="3542113" y="1442683"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E55C164A-D158-44C3-992D-9E05203EC78A}">
@@ -6965,8 +7131,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3658286" y="1679499"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="3659790" y="1679626"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7028,8 +7194,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3658286" y="1679499"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="3659790" y="1679626"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F53E32E6-1B95-4DC0-8746-5EC314B7E0ED}">
@@ -7039,8 +7205,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3540657" y="1923112"/>
-          <a:ext cx="588146" cy="304516"/>
+          <a:off x="3542113" y="1923339"/>
+          <a:ext cx="588388" cy="304641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7082,12 +7248,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="42971" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="400050">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7100,14 +7266,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="900" kern="1200"/>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
             <a:t>BGP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3540657" y="1923112"/>
-        <a:ext cx="588146" cy="304516"/>
+        <a:off x="3542113" y="1923339"/>
+        <a:ext cx="588388" cy="304641"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{71CEC9A2-8043-42B2-8F31-BF0E6BE9F92A}">
@@ -7117,8 +7283,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3658286" y="2159958"/>
-          <a:ext cx="529332" cy="101505"/>
+          <a:off x="3659790" y="2160283"/>
+          <a:ext cx="529549" cy="101547"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7180,8 +7346,163 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3658286" y="2159958"/>
-        <a:ext cx="529332" cy="101505"/>
+        <a:off x="3659790" y="2160283"/>
+        <a:ext cx="529549" cy="101547"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{9B6B8576-2E1F-4286-BDE0-9C8BAC7DBD7E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3147416" y="481369"/>
+          <a:ext cx="588388" cy="304641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5080" tIns="5080" rIns="5080" bIns="42988" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-AR" sz="800" kern="1200"/>
+            <a:t>Desconocida</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3147416" y="481369"/>
+        <a:ext cx="588388" cy="304641"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{18CBFCD1-65B0-495C-8F36-17F65655C045}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3265094" y="718313"/>
+          <a:ext cx="529549" cy="101547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="3810" rIns="15240" bIns="3810" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="266700">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-AR" sz="600" kern="1200"/>
+            <a:t>255</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3265094" y="718313"/>
+        <a:ext cx="529549" cy="101547"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -9693,35 +10014,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F771B50-66F1-467B-8B91-06AF5FDE8625}" name="Tabla2" displayName="Tabla2" ref="A1:G2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F771B50-66F1-467B-8B91-06AF5FDE8625}" name="Tabla2" displayName="Tabla2" ref="A1:G2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:G2" xr:uid="{2F771B50-66F1-467B-8B91-06AF5FDE8625}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C6AB6C44-5018-42A1-8569-9E4D46008BC5}" name="red" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E0B0A042-64DB-4300-9411-F8A74766AB04}" name="solicitada" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{5C58E59E-4E0C-434B-ADA9-E0E95F70B1EF}" name="disponible" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{9218950F-4887-4FDC-AF30-55C5898488BA}" name="bits" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{6FC035BE-EADD-4667-8C9D-6585CEF31CFF}" name="cidr" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{8ABA4D5C-6F37-4E62-AB17-D21A500FBCDC}" name="host" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{56BF9C24-6D73-468E-BEA6-B463943BC250}" name="next-hop" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{C6AB6C44-5018-42A1-8569-9E4D46008BC5}" name="red" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{E0B0A042-64DB-4300-9411-F8A74766AB04}" name="solicitada" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{5C58E59E-4E0C-434B-ADA9-E0E95F70B1EF}" name="disponible" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{9218950F-4887-4FDC-AF30-55C5898488BA}" name="bits" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{6FC035BE-EADD-4667-8C9D-6585CEF31CFF}" name="cidr" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{8ABA4D5C-6F37-4E62-AB17-D21A500FBCDC}" name="host" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{56BF9C24-6D73-468E-BEA6-B463943BC250}" name="next-hop" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD61EF7D-8DA1-41B9-9EF9-850A4BCF3870}" name="Tabla3" displayName="Tabla3" ref="A5:J10" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD61EF7D-8DA1-41B9-9EF9-850A4BCF3870}" name="Tabla3" displayName="Tabla3" ref="A5:J10" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A5:J10" xr:uid="{BD61EF7D-8DA1-41B9-9EF9-850A4BCF3870}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3B2BABE1-2DA1-4465-8B7E-899B7A83BC3A}" name="DTO" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{54545EFD-85FD-44BB-903F-3969F59F268E}" name="HOSTS" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{BD3B263E-8BD5-42DC-A8F3-4406423FEB9E}" name="Bits" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{9580F611-0208-42FB-BEFC-77CD732CC975}" name="CIDR" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{3C911C86-9F75-4873-8F81-E77060A1246A}" name="hosts2" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3B2BABE1-2DA1-4465-8B7E-899B7A83BC3A}" name="DTO" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{54545EFD-85FD-44BB-903F-3969F59F268E}" name="HOSTS" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{BD3B263E-8BD5-42DC-A8F3-4406423FEB9E}" name="Bits" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{9580F611-0208-42FB-BEFC-77CD732CC975}" name="CIDR" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{3C911C86-9F75-4873-8F81-E77060A1246A}" name="hosts2" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{75CCFFA8-4133-44BD-B450-374E375D8B2D}" name="RED"/>
     <tableColumn id="7" xr3:uid="{ED6F2FB8-7C8C-4BF7-B392-F02A9CAF94E6}" name="primer IP "/>
     <tableColumn id="8" xr3:uid="{6B891C26-911A-4328-A17B-A8B1E2C8451F}" name="ultima IP"/>
     <tableColumn id="9" xr3:uid="{34624768-CD8C-4D48-9693-A8E0B9678453}" name="BROADCAST"/>
-    <tableColumn id="10" xr3:uid="{9FB144F9-8C52-4261-BC51-706438AC0A00}" name="Mask" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{9FB144F9-8C52-4261-BC51-706438AC0A00}" name="Mask" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12110,8 +12431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E410DA1-3782-4158-8F8D-6DB4F797F961}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>